<commit_message>
Them database vao source
</commit_message>
<xml_diff>
--- a/trunk/document/Github/github_document.xlsx
+++ b/trunk/document/Github/github_document.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hung\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\denti\DentiReposory\DentiRepository\DentiRepository\trunk\document\Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Clone" sheetId="2" r:id="rId2"/>
     <sheet name="Comit" sheetId="5" r:id="rId3"/>
     <sheet name="Pull" sheetId="6" r:id="rId4"/>
+    <sheet name="Revert" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
   <si>
     <t>No.</t>
   </si>
@@ -77,9 +78,6 @@
     <t>Nhập url vào và bấm OK (Click vào đây để copy url)</t>
   </si>
   <si>
-    <t>Cài đặt totoirse git</t>
-  </si>
-  <si>
     <t>Comit</t>
   </si>
   <si>
@@ -92,9 +90,6 @@
     <t>Đã clone.</t>
   </si>
   <si>
-    <t>Cài đặt totoirse git.</t>
-  </si>
-  <si>
     <t>Đã clone, đảm bảo tất cả các file cần up đều nằm trong thư mục đã clone về.</t>
   </si>
   <si>
@@ -125,9 +120,6 @@
     <t>Pull</t>
   </si>
   <si>
-    <t>Download file từ repository github</t>
-  </si>
-  <si>
     <t>Click phải vào file hoặc thư mục chọn totoirse git -&gt; pull</t>
   </si>
   <si>
@@ -138,6 +130,39 @@
   </si>
   <si>
     <t>https://github.com/HungDuongUIT/DentiRepository</t>
+  </si>
+  <si>
+    <t>Cài đặt totoirse git, tạo tài khoản github</t>
+  </si>
+  <si>
+    <t>Cài đặt totoirse git, tạo tài khoản github.</t>
+  </si>
+  <si>
+    <t>Authorize</t>
+  </si>
+  <si>
+    <t>Cấp quyền với repository</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Download những gì thay đổi từ repository github về máy.</t>
+  </si>
+  <si>
+    <t>Revert</t>
+  </si>
+  <si>
+    <t>Lấy lại source, file ban đầu khi mà việc chỉnh sửa bị vấn đề</t>
+  </si>
+  <si>
+    <t>Download những gì thay đổi mới từ repository github về máy.</t>
+  </si>
+  <si>
+    <t>Click phải vào file hoặc thư mục chọn totoirse git -&gt; revert</t>
+  </si>
+  <si>
+    <t>Lấy lại source, file ban đầu khi mà việc chỉnh sửa bị vấn đề.</t>
   </si>
 </sst>
 </file>
@@ -593,9 +618,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -620,6 +642,129 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -629,85 +774,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -716,77 +807,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1750,6 +1775,124 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6568</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9197</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>112657</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>66347</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="616168" y="6286172"/>
+          <a:ext cx="13012464" cy="7105650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>708933</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>1951</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>436790</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>55790</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6195333" y="10088926"/>
+          <a:ext cx="2271032" cy="244339"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2013,10 +2156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F17"/>
+  <dimension ref="B1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,7 +2177,7 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2051,159 +2194,184 @@
       <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F3" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="C4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>17</v>
+      <c r="C5" s="10" t="s">
+        <v>3</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>3</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>31</v>
+      <c r="C6" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>4</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>5</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="13"/>
+      <c r="C8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>6</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="13"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>7</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="13"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>8</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>9</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="13"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>10</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>11</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>12</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="13"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>13</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="9">
+      <c r="E16" s="10"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="7">
         <v>14</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="14"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="7">
+        <v>15</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2214,231 +2382,231 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="37" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="29" style="37" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="29" style="26" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="56"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="23">
         <v>42866</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="57"/>
+      <c r="C4" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
     </row>
     <row r="5" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="58"/>
+      <c r="C5" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="51"/>
     </row>
     <row r="6" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="60"/>
     </row>
     <row r="7" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="59"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="63"/>
     </row>
     <row r="8" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41">
+      <c r="B8" s="30">
         <v>1</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="60"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
     </row>
     <row r="9" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="41">
+      <c r="B9" s="30">
         <v>2</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="60"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54"/>
     </row>
     <row r="10" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="61">
+      <c r="B10" s="43">
         <v>3</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="64"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="57"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="43"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="43"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="43"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="43"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="43"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="43"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="43"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="43"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="43"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="43"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="43"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="39"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="23"/>
+      <c r="B25" s="19"/>
     </row>
     <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="67" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="68" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="38" t="s">
+      <c r="B68" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="108" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="38" t="s">
+      <c r="B109" s="27" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25:D1048576">
@@ -2461,239 +2629,239 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E192"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="26" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="37" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="29" style="37" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" width="9.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="29" style="26" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="26"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="56"/>
+      <c r="C2" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="23">
         <v>42866</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
+    </row>
+    <row r="5" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="51"/>
+    </row>
+    <row r="6" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="70"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="72"/>
+    </row>
+    <row r="7" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="62"/>
+      <c r="E7" s="63"/>
+    </row>
+    <row r="8" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="38">
+        <v>1</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="64"/>
+      <c r="E8" s="65"/>
+    </row>
+    <row r="9" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="38">
+        <v>2</v>
+      </c>
+      <c r="C9" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="57"/>
-    </row>
-    <row r="5" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="47" t="s">
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
+    </row>
+    <row r="10" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="38">
+        <v>3</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="66"/>
+      <c r="E10" s="67"/>
+    </row>
+    <row r="11" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="38">
         <v>4</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="58"/>
-    </row>
-    <row r="6" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="48"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="68"/>
-    </row>
-    <row r="7" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="59"/>
-    </row>
-    <row r="8" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="51">
-        <v>1</v>
-      </c>
-      <c r="C8" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="66"/>
-      <c r="E8" s="69"/>
-    </row>
-    <row r="9" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="51">
-        <v>2</v>
-      </c>
-      <c r="C9" s="66" t="s">
+      <c r="C11" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="69"/>
-    </row>
-    <row r="10" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="51">
-        <v>3</v>
-      </c>
-      <c r="C10" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="67"/>
-      <c r="E10" s="70"/>
-    </row>
-    <row r="11" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="51">
-        <v>4</v>
-      </c>
-      <c r="C11" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="67"/>
-      <c r="E11" s="70"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="67"/>
     </row>
     <row r="12" spans="2:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="71">
+      <c r="B12" s="45">
         <v>5</v>
       </c>
-      <c r="C12" s="72" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="72"/>
-      <c r="E12" s="73"/>
+      <c r="C12" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="68"/>
+      <c r="E12" s="69"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="52"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="52"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="52"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="52"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="52"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="52"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="52"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="52"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="52"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="52"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="53"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="53"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="54"/>
+      <c r="B25" s="41"/>
     </row>
     <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="42" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="67" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="68" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="55" t="s">
+      <c r="B68" s="42" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="108" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="55" t="s">
+      <c r="B109" s="42" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="149" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="150" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="55" t="s">
-        <v>28</v>
+      <c r="B150" s="42" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="191" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="192" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B192" s="55" t="s">
-        <v>29</v>
+      <c r="B192" s="42" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2731,209 +2899,437 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E68"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="26" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="37" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="29" style="37" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" width="9.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="29" style="26" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="26"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="56"/>
+      <c r="C2" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="23">
         <v>42866</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="57"/>
+      <c r="C4" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
     </row>
     <row r="5" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="58"/>
+      <c r="C5" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="51"/>
     </row>
     <row r="6" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="48"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="68"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="72"/>
     </row>
     <row r="7" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="59"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="63"/>
     </row>
     <row r="8" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="51">
+      <c r="B8" s="38">
         <v>1</v>
       </c>
-      <c r="C8" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="66"/>
-      <c r="E8" s="69"/>
+      <c r="C8" s="73" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="64"/>
+      <c r="E8" s="65"/>
     </row>
     <row r="9" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="51">
+      <c r="B9" s="38">
         <v>2</v>
       </c>
-      <c r="C9" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="69"/>
+      <c r="C9" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="52"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="52"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="52"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="52"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="52"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="52"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="52"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="52"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="52"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="52"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="52"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="52"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="52"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="53"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="53"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="54"/>
+      <c r="B25" s="41"/>
     </row>
     <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="42" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="67" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="68" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="55" t="s">
+      <c r="B68" s="42" t="s">
         <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25:D1048576">
+      <formula1>"PRIMARY KEY, NULL, NOT NULL, FOREIGN KEY"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B8" location="Pull!B27" display="Pull!B27"/>
+    <hyperlink ref="B9" location="Pull!B68" display="Pull!B68"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="29" style="26" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="22"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
+    </row>
+    <row r="3" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="23">
+        <v>42866</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
+    </row>
+    <row r="5" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="51"/>
+    </row>
+    <row r="6" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="70"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="72"/>
+    </row>
+    <row r="7" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="62"/>
+      <c r="E7" s="63"/>
+    </row>
+    <row r="8" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="38">
+        <v>1</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="64"/>
+      <c r="E8" s="65"/>
+    </row>
+    <row r="9" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="38">
+        <v>2</v>
+      </c>
+      <c r="C9" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="39"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="39"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="39"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="39"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="39"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="39"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="39"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="39"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="39"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="39"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="39"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="39"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="39"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="40"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="40"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="41"/>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="42" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>